<commit_message>
Added comments to Students.
</commit_message>
<xml_diff>
--- a/Students/Resources/Report1.xlsx
+++ b/Students/Resources/Report1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\learn\C#\EPAM\EPAM_Task6\EPAM_Task6\Students\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48C61029-4CEA-438D-97F5-754784090DBF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C5E99AC-F804-4056-81E5-4C02A84AFEEB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="8304" xr2:uid="{35617191-F315-4048-8243-739946202327}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="8304" xr2:uid="{4CFF25D0-E738-450B-9F74-D907F55EC194}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -451,7 +451,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9022DA20-2661-4AE0-8F98-D190E8A1AAED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F7F03E-855F-4192-A491-3D5E8AC81D42}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Added tests for ORM.
</commit_message>
<xml_diff>
--- a/Students/Resources/Report1.xlsx
+++ b/Students/Resources/Report1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\learn\C#\EPAM\EPAM_Task6\EPAM_Task6\Students\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C5E99AC-F804-4056-81E5-4C02A84AFEEB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F18B3DF-702C-402C-80B0-A429C42B0884}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="8304" xr2:uid="{4CFF25D0-E738-450B-9F74-D907F55EC194}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="8304" xr2:uid="{660AF674-88A9-4638-A128-915A2B38484E}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Session</t>
   </si>
@@ -45,61 +45,31 @@
     <t>Mark</t>
   </si>
   <si>
-    <t>IP-32</t>
-  </si>
-  <si>
-    <t>Shyshkavets Pavel Sergeevich</t>
-  </si>
-  <si>
-    <t>OOP</t>
+    <t>IP-21</t>
+  </si>
+  <si>
+    <t>Artem Lukavtsov Gennadevich</t>
+  </si>
+  <si>
+    <t>Math</t>
   </si>
   <si>
     <t>Exam</t>
   </si>
   <si>
+    <t>History</t>
+  </si>
+  <si>
     <t>Credit</t>
   </si>
   <si>
     <t>Passed</t>
   </si>
   <si>
-    <t>Reita Match Sergeevna</t>
-  </si>
-  <si>
-    <t>Not Passes</t>
-  </si>
-  <si>
-    <t>IP-21</t>
-  </si>
-  <si>
-    <t>Artem Lukavtsov Gennadevich</t>
-  </si>
-  <si>
-    <t>Math</t>
-  </si>
-  <si>
-    <t>History</t>
-  </si>
-  <si>
     <t>Borisenko Ivan Sergeevich</t>
   </si>
   <si>
     <t>Not Passed</t>
-  </si>
-  <si>
-    <t>IP-31</t>
-  </si>
-  <si>
-    <t>Chaykov Andey Vasllyevich</t>
-  </si>
-  <si>
-    <t>SUBD</t>
-  </si>
-  <si>
-    <t>TVIMS</t>
-  </si>
-  <si>
-    <t>Palatkin Daniil Aleksandrovich</t>
   </si>
 </sst>
 </file>
@@ -451,8 +421,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F7F03E-855F-4192-A491-3D5E8AC81D42}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8554C4F-A8D5-4E3D-AC45-FB33CE6B68BF}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -483,19 +453,19 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -503,19 +473,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -523,13 +493,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -543,13 +513,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -558,168 +528,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A2:F13">
+  <sortState ref="A2:F5">
     <sortCondition ref="D1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>